<commit_message>
change Factura y Caja
add totales
</commit_message>
<xml_diff>
--- a/files/CajaSirius.xlsx
+++ b/files/CajaSirius.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t>No. Factura</t>
   </si>
@@ -35,9 +35,6 @@
     <t>No. Cliente</t>
   </si>
   <si>
-    <t>Descripci</t>
-  </si>
-  <si>
     <t>Fecha</t>
   </si>
   <si>
@@ -89,7 +86,67 @@
     <t>Importe</t>
   </si>
   <si>
-    <t>xxx</t>
+    <t>CONSTRUCCIONES LACAYO FIALLOS</t>
+  </si>
+  <si>
+    <t>TORRES IN SITU, SA.</t>
+  </si>
+  <si>
+    <t>CONSTRUVAL</t>
+  </si>
+  <si>
+    <t>MEGA INVERSIONES SA</t>
+  </si>
+  <si>
+    <t>SINSA</t>
+  </si>
+  <si>
+    <t>ALBA-EQUIPOS,S.A.</t>
+  </si>
+  <si>
+    <t>PUMA ENERGY BAHAMAS, S.A.</t>
+  </si>
+  <si>
+    <t>Descripcion</t>
+  </si>
+  <si>
+    <t>R/C16512</t>
+  </si>
+  <si>
+    <t>R/C16513</t>
+  </si>
+  <si>
+    <t>R/C16517</t>
+  </si>
+  <si>
+    <t>R/C16518</t>
+  </si>
+  <si>
+    <t>R/C16519</t>
+  </si>
+  <si>
+    <t>R/C16520</t>
+  </si>
+  <si>
+    <t>APLICACION DE AN1846 A F96148</t>
+  </si>
+  <si>
+    <t>R/C16521</t>
+  </si>
+  <si>
+    <t>APLICAR N/C1841</t>
+  </si>
+  <si>
+    <t>aplicar n/c1798</t>
+  </si>
+  <si>
+    <t>APLICAR AN F.92162</t>
+  </si>
+  <si>
+    <t>APLICAR AN F.91327</t>
+  </si>
+  <si>
+    <t>AN1846</t>
   </si>
 </sst>
 </file>
@@ -140,10 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -424,144 +483,693 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W2"/>
+  <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="8.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" style="2"/>
+    <col min="9" max="9" width="7.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="11.28515625" style="2"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="2">
+        <v>49</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P2" s="2">
+        <v>93799</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="2">
+        <v>49</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G3" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P3" s="2">
+        <v>93806</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2">
+        <v>49</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P4" s="2">
+        <v>93807</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
+        <v>49</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P5" s="2">
+        <v>93813</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="2">
+        <v>49</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P6" s="2">
+        <v>93820</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="2">
+        <v>49</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="3">
+        <v>42781</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4">
+        <v>230609.3</v>
+      </c>
+      <c r="P7" s="2">
+        <v>93830</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="2">
+        <v>49</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G8" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P8" s="2">
+        <v>93824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="2">
+        <v>49</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G9" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P9" s="2">
+        <v>93826</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="2">
+        <v>49</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G10" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P10" s="2">
+        <v>93827</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="2">
+        <v>49</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P11" s="2">
+        <v>93828</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="2">
+        <v>49</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D12" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G12" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P12" s="2">
+        <v>93829</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="2">
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G13" s="4">
+        <v>192185.76</v>
+      </c>
+      <c r="P13" s="2">
+        <v>93832</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="2">
+        <v>2139</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G14" s="4">
+        <v>73698.22</v>
+      </c>
+      <c r="P14" s="2">
+        <v>94298</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="2">
+        <v>2139</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G15" s="4">
+        <v>73698.22</v>
+      </c>
+      <c r="P15" s="2">
+        <v>94309</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="2">
+        <v>2139</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G16" s="4">
+        <v>73698.22</v>
+      </c>
+      <c r="P16" s="2">
+        <v>94325</v>
+      </c>
+    </row>
+    <row r="17" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="2">
+        <v>3488</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G17" s="4">
+        <v>11802.24</v>
+      </c>
+      <c r="P17" s="2">
+        <v>96160</v>
+      </c>
+    </row>
+    <row r="18" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G18" s="4">
+        <v>14752.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G19" s="4">
+        <v>2134.67</v>
+      </c>
+      <c r="P19" s="2">
+        <v>96113</v>
+      </c>
+    </row>
+    <row r="20" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2134.67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2">
+        <v>695</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D21" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="2">
         <v>0</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="W2" s="1"/>
+      <c r="P21" s="2">
+        <v>96148</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2">
+        <v>695</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D22" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="2">
+        <v>0</v>
+      </c>
+      <c r="P22" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="G23" s="4">
+        <v>5182.1099999999997</v>
+      </c>
+      <c r="P23" s="2">
+        <v>96114</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="2">
+        <v>0</v>
+      </c>
+      <c r="P24" s="2">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="G25" s="2">
+        <v>0</v>
+      </c>
+      <c r="P25" s="2">
+        <v>96114</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="2">
+        <v>0</v>
+      </c>
+      <c r="P26" s="2">
+        <v>96114</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2">
+        <v>6255</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="3">
+        <v>42782</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2">
+        <v>3119</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D28" s="3">
+        <v>42783</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="2">
+        <v>0</v>
+      </c>
+      <c r="P28" s="2">
+        <v>92162</v>
+      </c>
+    </row>
+    <row r="29" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2">
+        <v>3119</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="3">
+        <v>42783</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="2">
+        <v>0</v>
+      </c>
+      <c r="P29" s="2">
+        <v>92162</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2">
+        <v>1237</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="3">
+        <v>42783</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G30" s="2">
+        <v>0</v>
+      </c>
+      <c r="P30" s="2">
+        <v>91327</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2">
+        <v>1237</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D31" s="3">
+        <v>42783</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="G31" s="2">
+        <v>0</v>
+      </c>
+      <c r="P31" s="2">
+        <v>91327</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
cahnge 09/marzo part 1
</commit_message>
<xml_diff>
--- a/files/CajaSirius.xlsx
+++ b/files/CajaSirius.xlsx
@@ -197,12 +197,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -485,8 +486,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,11 +512,11 @@
     <col min="18" max="18" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="8.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="22" max="16384" width="11.28515625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -580,7 +581,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B2" s="2">
         <v>49</v>
       </c>
@@ -599,8 +600,11 @@
       <c r="P2" s="2">
         <v>93799</v>
       </c>
-    </row>
-    <row r="3" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U2" s="5">
+        <v>53454.6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
         <v>49</v>
       </c>
@@ -619,8 +623,11 @@
       <c r="P3" s="2">
         <v>93806</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U3" s="5">
+        <v>46369.98</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B4" s="2">
         <v>49</v>
       </c>
@@ -639,8 +646,11 @@
       <c r="P4" s="2">
         <v>93807</v>
       </c>
-    </row>
-    <row r="5" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U4" s="5">
+        <v>46247.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
         <v>49</v>
       </c>
@@ -659,8 +669,11 @@
       <c r="P5" s="2">
         <v>93813</v>
       </c>
-    </row>
-    <row r="6" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U5" s="5">
+        <v>3165.42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B6" s="2">
         <v>49</v>
       </c>
@@ -679,8 +692,11 @@
       <c r="P6" s="2">
         <v>93820</v>
       </c>
-    </row>
-    <row r="7" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U6" s="5">
+        <v>74547.31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B7" s="2">
         <v>49</v>
       </c>
@@ -699,8 +715,11 @@
       <c r="P7" s="2">
         <v>93830</v>
       </c>
-    </row>
-    <row r="8" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U7" s="5">
+        <v>6824.74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B8" s="2">
         <v>49</v>
       </c>
@@ -719,8 +738,11 @@
       <c r="P8" s="2">
         <v>93824</v>
       </c>
-    </row>
-    <row r="9" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U8" s="5">
+        <v>19806.45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B9" s="2">
         <v>49</v>
       </c>
@@ -739,8 +761,11 @@
       <c r="P9" s="2">
         <v>93826</v>
       </c>
-    </row>
-    <row r="10" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U9" s="5">
+        <v>21141.599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
         <v>49</v>
       </c>
@@ -759,8 +784,11 @@
       <c r="P10" s="2">
         <v>93827</v>
       </c>
-    </row>
-    <row r="11" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U10" s="5">
+        <v>67971.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B11" s="2">
         <v>49</v>
       </c>
@@ -779,8 +807,11 @@
       <c r="P11" s="2">
         <v>93828</v>
       </c>
-    </row>
-    <row r="12" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U11" s="5">
+        <v>55138.22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B12" s="2">
         <v>49</v>
       </c>
@@ -799,8 +830,11 @@
       <c r="P12" s="2">
         <v>93829</v>
       </c>
-    </row>
-    <row r="13" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U12" s="5">
+        <v>26574.65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B13" s="2">
         <v>49</v>
       </c>
@@ -819,8 +853,11 @@
       <c r="P13" s="2">
         <v>93832</v>
       </c>
-    </row>
-    <row r="14" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U13" s="5">
+        <v>1552.93</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B14" s="2">
         <v>2139</v>
       </c>
@@ -839,8 +876,11 @@
       <c r="P14" s="2">
         <v>94298</v>
       </c>
-    </row>
-    <row r="15" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U14" s="5">
+        <v>30988.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B15" s="2">
         <v>2139</v>
       </c>
@@ -859,8 +899,11 @@
       <c r="P15" s="2">
         <v>94309</v>
       </c>
-    </row>
-    <row r="16" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U15" s="5">
+        <v>14820.46</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="B16" s="2">
         <v>2139</v>
       </c>
@@ -879,8 +922,11 @@
       <c r="P16" s="2">
         <v>94325</v>
       </c>
-    </row>
-    <row r="17" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U16" s="5">
+        <v>27889.46</v>
+      </c>
+    </row>
+    <row r="17" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B17" s="2">
         <v>3488</v>
       </c>
@@ -899,8 +945,11 @@
       <c r="P17" s="2">
         <v>96160</v>
       </c>
-    </row>
-    <row r="18" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U17" s="5">
+        <v>11802.24</v>
+      </c>
+    </row>
+    <row r="18" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B18" s="2">
         <v>6255</v>
       </c>
@@ -916,8 +965,11 @@
       <c r="G18" s="4">
         <v>14752.8</v>
       </c>
-    </row>
-    <row r="19" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U18" s="5">
+        <v>14752.8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B19" s="2">
         <v>6255</v>
       </c>
@@ -936,8 +988,11 @@
       <c r="P19" s="2">
         <v>96113</v>
       </c>
-    </row>
-    <row r="20" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U19" s="5">
+        <v>2134.64</v>
+      </c>
+    </row>
+    <row r="20" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B20" s="2">
         <v>6255</v>
       </c>
@@ -953,8 +1008,11 @@
       <c r="G20" s="4">
         <v>2134.67</v>
       </c>
-    </row>
-    <row r="21" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U20">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="21" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B21" s="2">
         <v>695</v>
       </c>
@@ -973,8 +1031,11 @@
       <c r="P21" s="2">
         <v>96148</v>
       </c>
-    </row>
-    <row r="22" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U21" s="5">
+        <v>1056.97</v>
+      </c>
+    </row>
+    <row r="22" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>695</v>
       </c>
@@ -993,8 +1054,11 @@
       <c r="P22" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="23" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U22" s="5">
+        <v>-1056.97</v>
+      </c>
+    </row>
+    <row r="23" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B23" s="2">
         <v>6255</v>
       </c>
@@ -1013,8 +1077,11 @@
       <c r="P23" s="2">
         <v>96114</v>
       </c>
-    </row>
-    <row r="24" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U23" s="5">
+        <v>5182.1099999999997</v>
+      </c>
+    </row>
+    <row r="24" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B24" s="2">
         <v>6255</v>
       </c>
@@ -1033,8 +1100,11 @@
       <c r="P24" s="2">
         <v>1841</v>
       </c>
-    </row>
-    <row r="25" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U24">
+        <v>-279.75</v>
+      </c>
+    </row>
+    <row r="25" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B25" s="2">
         <v>6255</v>
       </c>
@@ -1053,8 +1123,11 @@
       <c r="P25" s="2">
         <v>96114</v>
       </c>
-    </row>
-    <row r="26" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U25">
+        <v>279.75</v>
+      </c>
+    </row>
+    <row r="26" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B26" s="2">
         <v>6255</v>
       </c>
@@ -1073,8 +1146,11 @@
       <c r="P26" s="2">
         <v>96114</v>
       </c>
-    </row>
-    <row r="27" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U26" s="5">
+        <v>1324.42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B27" s="2">
         <v>6255</v>
       </c>
@@ -1090,8 +1166,11 @@
       <c r="G27" s="2">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U27" s="5">
+        <v>-1324.42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B28" s="2">
         <v>3119</v>
       </c>
@@ -1110,8 +1189,11 @@
       <c r="P28" s="2">
         <v>92162</v>
       </c>
-    </row>
-    <row r="29" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U28">
+        <v>732.09</v>
+      </c>
+    </row>
+    <row r="29" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B29" s="2">
         <v>3119</v>
       </c>
@@ -1130,8 +1212,11 @@
       <c r="P29" s="2">
         <v>92162</v>
       </c>
-    </row>
-    <row r="30" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U29">
+        <v>-732.09</v>
+      </c>
+    </row>
+    <row r="30" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B30" s="2">
         <v>1237</v>
       </c>
@@ -1150,8 +1235,11 @@
       <c r="P30" s="2">
         <v>91327</v>
       </c>
-    </row>
-    <row r="31" spans="2:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="U30" s="5">
+        <v>43812.12</v>
+      </c>
+    </row>
+    <row r="31" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B31" s="2">
         <v>1237</v>
       </c>
@@ -1169,6 +1257,9 @@
       </c>
       <c r="P31" s="2">
         <v>91327</v>
+      </c>
+      <c r="U31" s="5">
+        <v>-43812.12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>